<commit_message>
updates on xml format and new relevant info found
</commit_message>
<xml_diff>
--- a/scicura_files/rules_ppm.xlsx
+++ b/scicura_files/rules_ppm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppm/Documents/Collaborations/scicura/scicura_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pporras/Documents/Collaborations/scicura_mapping/scicura2psi/scicura_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAA2A8F-28D9-074D-BB79-F013ABFBC10F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="2900" windowWidth="32900" windowHeight="18600" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Int. methods vs part. methods " sheetId="1" r:id="rId1"/>
@@ -19,23 +20,23 @@
     <sheet name="int. methods vs host organism" sheetId="5" r:id="rId5"/>
     <sheet name="Scicura vs Intact host org." sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="514">
   <si>
     <t>Interaction detection method</t>
   </si>
@@ -775,9 +776,6 @@
     <t>taxid:9606(BxPC-3 cell)</t>
   </si>
   <si>
-    <t>human-bpxc3</t>
-  </si>
-  <si>
     <t>taxid:9606(DLD-1 cell)</t>
   </si>
   <si>
@@ -1138,15 +1136,9 @@
     <t>partdetmet_mi_B</t>
   </si>
   <si>
-    <t>inferred by curator</t>
-  </si>
-  <si>
     <t>primer specific pcr</t>
   </si>
   <si>
-    <t>MI:0364</t>
-  </si>
-  <si>
     <t>MI:0088</t>
   </si>
   <si>
@@ -1583,12 +1575,15 @@
   </si>
   <si>
     <t>psi-mi:"MI:0929"(northern blot)</t>
+  </si>
+  <si>
+    <t>human-bxpc3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1979,11 +1974,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1999,25 +1994,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2025,22 +2020,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2048,22 +2043,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2071,22 +2066,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2094,45 +2089,45 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2140,22 +2135,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2163,22 +2158,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2186,22 +2181,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2209,137 +2204,137 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>420</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -2349,7 +2344,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2372,10 +2367,10 @@
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2538,10 +2533,10 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D21" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2552,10 +2547,10 @@
         <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D22" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2566,10 +2561,10 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D23" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2580,10 +2575,10 @@
         <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D24" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2594,10 +2589,10 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D25" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2608,10 +2603,10 @@
         <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D26" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2622,10 +2617,10 @@
         <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D27" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2636,10 +2631,10 @@
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D28" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2650,10 +2645,10 @@
         <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D29" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2664,10 +2659,10 @@
         <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D30" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2678,10 +2673,10 @@
         <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D31" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2692,10 +2687,10 @@
         <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D32" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2706,10 +2701,10 @@
         <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D33" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2720,10 +2715,10 @@
         <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D34" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2734,10 +2729,10 @@
         <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D35" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2748,10 +2743,10 @@
         <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D36" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2762,10 +2757,10 @@
         <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D37" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2776,10 +2771,10 @@
         <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D38" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2790,10 +2785,10 @@
         <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D39" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2804,10 +2799,10 @@
         <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D40" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2818,10 +2813,10 @@
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D41" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2832,10 +2827,10 @@
         <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D42" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2846,10 +2841,10 @@
         <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D43" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2860,10 +2855,10 @@
         <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D44" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2874,10 +2869,10 @@
         <v>55</v>
       </c>
       <c r="C45" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D45" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2888,10 +2883,10 @@
         <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D46" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2902,10 +2897,10 @@
         <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D47" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2916,10 +2911,10 @@
         <v>58</v>
       </c>
       <c r="C48" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D48" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2930,10 +2925,10 @@
         <v>59</v>
       </c>
       <c r="C49" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D49" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2944,10 +2939,10 @@
         <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D50" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2958,10 +2953,10 @@
         <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D51" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2972,10 +2967,10 @@
         <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D52" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -2986,10 +2981,10 @@
         <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D53" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3000,10 +2995,10 @@
         <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D54" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3014,10 +3009,10 @@
         <v>65</v>
       </c>
       <c r="C55" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D55" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3028,10 +3023,10 @@
         <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D56" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3042,10 +3037,10 @@
         <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D57" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3056,10 +3051,10 @@
         <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D58" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3070,10 +3065,10 @@
         <v>69</v>
       </c>
       <c r="C59" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D59" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3084,10 +3079,10 @@
         <v>70</v>
       </c>
       <c r="C60" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D60" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3098,10 +3093,10 @@
         <v>71</v>
       </c>
       <c r="C61" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D61" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3112,10 +3107,10 @@
         <v>72</v>
       </c>
       <c r="C62" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D62" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3126,10 +3121,10 @@
         <v>73</v>
       </c>
       <c r="C63" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D63" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3140,10 +3135,10 @@
         <v>74</v>
       </c>
       <c r="C64" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D64" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3154,10 +3149,10 @@
         <v>75</v>
       </c>
       <c r="C65" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D65" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3168,10 +3163,10 @@
         <v>76</v>
       </c>
       <c r="C66" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D66" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3182,10 +3177,10 @@
         <v>77</v>
       </c>
       <c r="C67" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D67" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3196,10 +3191,10 @@
         <v>78</v>
       </c>
       <c r="C68" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D68" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3210,10 +3205,10 @@
         <v>79</v>
       </c>
       <c r="C69" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D69" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3224,10 +3219,10 @@
         <v>80</v>
       </c>
       <c r="C70" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D70" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3238,10 +3233,10 @@
         <v>81</v>
       </c>
       <c r="C71" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D71" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3252,10 +3247,10 @@
         <v>82</v>
       </c>
       <c r="C72" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D72" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3266,10 +3261,10 @@
         <v>83</v>
       </c>
       <c r="C73" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D73" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3280,10 +3275,10 @@
         <v>84</v>
       </c>
       <c r="C74" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D74" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3414,10 +3409,10 @@
         <v>100</v>
       </c>
       <c r="C90" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D90" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3428,10 +3423,10 @@
         <v>101</v>
       </c>
       <c r="C91" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D91" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3442,10 +3437,10 @@
         <v>102</v>
       </c>
       <c r="C92" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D92" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3456,10 +3451,10 @@
         <v>103</v>
       </c>
       <c r="C93" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D93" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3470,10 +3465,10 @@
         <v>104</v>
       </c>
       <c r="C94" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D94" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3484,10 +3479,10 @@
         <v>105</v>
       </c>
       <c r="C95" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D95" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3498,10 +3493,10 @@
         <v>106</v>
       </c>
       <c r="C96" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D96" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3512,10 +3507,10 @@
         <v>107</v>
       </c>
       <c r="C97" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D97" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3526,10 +3521,10 @@
         <v>108</v>
       </c>
       <c r="C98" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D98" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3540,10 +3535,10 @@
         <v>109</v>
       </c>
       <c r="C99" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D99" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3554,10 +3549,10 @@
         <v>110</v>
       </c>
       <c r="C100" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D100" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3568,10 +3563,10 @@
         <v>111</v>
       </c>
       <c r="C101" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D101" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3582,10 +3577,10 @@
         <v>112</v>
       </c>
       <c r="C102" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D102" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3596,10 +3591,10 @@
         <v>113</v>
       </c>
       <c r="C103" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D103" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3610,10 +3605,10 @@
         <v>114</v>
       </c>
       <c r="C104" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D104" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3624,10 +3619,10 @@
         <v>115</v>
       </c>
       <c r="C105" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D105" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3638,10 +3633,10 @@
         <v>116</v>
       </c>
       <c r="C106" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D106" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3652,10 +3647,10 @@
         <v>117</v>
       </c>
       <c r="C107" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D107" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3666,10 +3661,10 @@
         <v>118</v>
       </c>
       <c r="C108" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D108" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3680,10 +3675,10 @@
         <v>119</v>
       </c>
       <c r="C109" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D109" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3694,10 +3689,10 @@
         <v>120</v>
       </c>
       <c r="C110" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D110" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3708,10 +3703,10 @@
         <v>121</v>
       </c>
       <c r="C111" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D111" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3722,10 +3717,10 @@
         <v>122</v>
       </c>
       <c r="C112" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D112" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3736,10 +3731,10 @@
         <v>123</v>
       </c>
       <c r="C113" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D113" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3750,10 +3745,10 @@
         <v>124</v>
       </c>
       <c r="C114" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D114" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3764,10 +3759,10 @@
         <v>125</v>
       </c>
       <c r="C115" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D115" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3778,10 +3773,10 @@
         <v>126</v>
       </c>
       <c r="C116" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D116" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3792,10 +3787,10 @@
         <v>127</v>
       </c>
       <c r="C117" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D117" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3806,10 +3801,10 @@
         <v>128</v>
       </c>
       <c r="C118" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D118" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3820,10 +3815,10 @@
         <v>129</v>
       </c>
       <c r="C119" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D119" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3834,10 +3829,10 @@
         <v>130</v>
       </c>
       <c r="C120" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D120" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3848,10 +3843,10 @@
         <v>131</v>
       </c>
       <c r="C121" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D121" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3862,10 +3857,10 @@
         <v>132</v>
       </c>
       <c r="C122" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D122" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3876,10 +3871,10 @@
         <v>133</v>
       </c>
       <c r="C123" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D123" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3890,10 +3885,10 @@
         <v>134</v>
       </c>
       <c r="C124" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D124" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3904,10 +3899,10 @@
         <v>135</v>
       </c>
       <c r="C125" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D125" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3918,10 +3913,10 @@
         <v>136</v>
       </c>
       <c r="C126" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D126" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3932,10 +3927,10 @@
         <v>137</v>
       </c>
       <c r="C127" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D127" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3946,10 +3941,10 @@
         <v>138</v>
       </c>
       <c r="C128" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D128" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3960,10 +3955,10 @@
         <v>139</v>
       </c>
       <c r="C129" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D129" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3974,10 +3969,10 @@
         <v>140</v>
       </c>
       <c r="C130" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D130" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -3988,10 +3983,10 @@
         <v>141</v>
       </c>
       <c r="C131" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D131" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4002,10 +3997,10 @@
         <v>142</v>
       </c>
       <c r="C132" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D132" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4016,10 +4011,10 @@
         <v>143</v>
       </c>
       <c r="C133" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D133" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4030,10 +4025,10 @@
         <v>144</v>
       </c>
       <c r="C134" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D134" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4044,10 +4039,10 @@
         <v>145</v>
       </c>
       <c r="C135" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D135" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4058,10 +4053,10 @@
         <v>146</v>
       </c>
       <c r="C136" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D136" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4072,10 +4067,10 @@
         <v>147</v>
       </c>
       <c r="C137" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D137" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4086,10 +4081,10 @@
         <v>148</v>
       </c>
       <c r="C138" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D138" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4100,10 +4095,10 @@
         <v>149</v>
       </c>
       <c r="C139" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D139" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4114,10 +4109,10 @@
         <v>150</v>
       </c>
       <c r="C140" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D140" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4128,10 +4123,10 @@
         <v>151</v>
       </c>
       <c r="C141" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D141" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4142,10 +4137,10 @@
         <v>152</v>
       </c>
       <c r="C142" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D142" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4156,10 +4151,10 @@
         <v>153</v>
       </c>
       <c r="C143" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D143" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4170,10 +4165,10 @@
         <v>154</v>
       </c>
       <c r="C144" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D144" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4184,10 +4179,10 @@
         <v>155</v>
       </c>
       <c r="C145" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D145" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -4336,175 +4331,175 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://scicura.org/f/classid=1000206915"/>
-    <hyperlink ref="A3" r:id="rId2" display="http://scicura.org/f/classid=1000206992"/>
-    <hyperlink ref="A4" r:id="rId3" display="http://scicura.org/f/classid=1000281286"/>
-    <hyperlink ref="A5" r:id="rId4" display="http://scicura.org/f/classid=1000206991"/>
-    <hyperlink ref="A6" r:id="rId5" display="http://scicura.org/f/classid=1000206990"/>
-    <hyperlink ref="A7" r:id="rId6" display="http://scicura.org/f/classid=1000206922"/>
-    <hyperlink ref="A8" r:id="rId7" display="http://scicura.org/f/classid=1000206923"/>
-    <hyperlink ref="A9" r:id="rId8" display="http://scicura.org/f/classid=1000206920"/>
-    <hyperlink ref="A10" r:id="rId9" display="http://scicura.org/f/classid=1000280758"/>
-    <hyperlink ref="A11" r:id="rId10" display="http://scicura.org/f/classid=1000206919"/>
-    <hyperlink ref="A12" r:id="rId11" display="http://scicura.org/f/classid=1000206921"/>
-    <hyperlink ref="A13" r:id="rId12" display="http://scicura.org/f/classid=1000206918"/>
-    <hyperlink ref="A14" r:id="rId13" display="http://scicura.org/f/classid=1000206989"/>
-    <hyperlink ref="A15" r:id="rId14" display="http://scicura.org/f/classid=1000206988"/>
-    <hyperlink ref="A16" r:id="rId15" display="http://scicura.org/f/classid=1000206974"/>
-    <hyperlink ref="A17" r:id="rId16" display="http://scicura.org/f/classid=1000206975"/>
-    <hyperlink ref="A18" r:id="rId17" display="http://scicura.org/f/classid=1000206978"/>
-    <hyperlink ref="A19" r:id="rId18" display="http://scicura.org/f/classid=1000206979"/>
-    <hyperlink ref="A20" r:id="rId19" display="http://scicura.org/f/classid=1000281314"/>
-    <hyperlink ref="A21" r:id="rId20" display="http://scicura.org/f/classid=1000280939"/>
-    <hyperlink ref="A22" r:id="rId21" display="http://scicura.org/f/classid=1000280944"/>
-    <hyperlink ref="A23" r:id="rId22" display="http://scicura.org/f/classid=1000280959"/>
-    <hyperlink ref="A24" r:id="rId23" display="http://scicura.org/f/classid=1000280964"/>
-    <hyperlink ref="A25" r:id="rId24" display="http://scicura.org/f/classid=1000280920"/>
-    <hyperlink ref="A26" r:id="rId25" display="http://scicura.org/f/classid=1000280924"/>
-    <hyperlink ref="A27" r:id="rId26" display="http://scicura.org/f/classid=1000280926"/>
-    <hyperlink ref="A28" r:id="rId27" display="http://scicura.org/f/classid=1000280922"/>
-    <hyperlink ref="A29" r:id="rId28" display="http://scicura.org/f/classid=1000280937"/>
-    <hyperlink ref="A30" r:id="rId29" display="http://scicura.org/f/classid=1000280942"/>
-    <hyperlink ref="A31" r:id="rId30" display="http://scicura.org/f/classid=1000280957"/>
-    <hyperlink ref="A32" r:id="rId31" display="http://scicura.org/f/classid=1000280962"/>
-    <hyperlink ref="A33" r:id="rId32" display="http://scicura.org/f/classid=1000206952"/>
-    <hyperlink ref="A34" r:id="rId33" display="http://scicura.org/f/classid=1000206964"/>
-    <hyperlink ref="A35" r:id="rId34" display="http://scicura.org/f/classid=1000206970"/>
-    <hyperlink ref="A36" r:id="rId35" display="http://scicura.org/f/classid=1000206958"/>
-    <hyperlink ref="A37" r:id="rId36" display="http://scicura.org/f/classid=1000280935"/>
-    <hyperlink ref="A38" r:id="rId37" display="http://scicura.org/f/classid=1000280940"/>
-    <hyperlink ref="A39" r:id="rId38" display="http://scicura.org/f/classid=1000280955"/>
-    <hyperlink ref="A40" r:id="rId39" display="http://scicura.org/f/classid=1000280960"/>
-    <hyperlink ref="A41" r:id="rId40" display="http://scicura.org/f/classid=1000206950"/>
-    <hyperlink ref="A42" r:id="rId41" display="http://scicura.org/f/classid=1000206962"/>
-    <hyperlink ref="A43" r:id="rId42" display="http://scicura.org/f/classid=1000206968"/>
-    <hyperlink ref="A44" r:id="rId43" display="http://scicura.org/f/classid=1000206956"/>
-    <hyperlink ref="A45" r:id="rId44" display="http://scicura.org/f/classid=1000280938"/>
-    <hyperlink ref="A46" r:id="rId45" display="http://scicura.org/f/classid=1000280943"/>
-    <hyperlink ref="A47" r:id="rId46" display="http://scicura.org/f/classid=1000280958"/>
-    <hyperlink ref="A48" r:id="rId47" display="http://scicura.org/f/classid=1000280963"/>
-    <hyperlink ref="A49" r:id="rId48" display="http://scicura.org/f/classid=1000280919"/>
-    <hyperlink ref="A50" r:id="rId49" display="http://scicura.org/f/classid=1000280923"/>
-    <hyperlink ref="A51" r:id="rId50" display="http://scicura.org/f/classid=1000280925"/>
-    <hyperlink ref="A52" r:id="rId51" display="http://scicura.org/f/classid=1000280921"/>
-    <hyperlink ref="A53" r:id="rId52" display="http://scicura.org/f/classid=1000280936"/>
-    <hyperlink ref="A54" r:id="rId53" display="http://scicura.org/f/classid=1000280941"/>
-    <hyperlink ref="A55" r:id="rId54" display="http://scicura.org/f/classid=1000280956"/>
-    <hyperlink ref="A56" r:id="rId55" display="http://scicura.org/f/classid=1000280961"/>
-    <hyperlink ref="A57" r:id="rId56" display="http://scicura.org/f/classid=1000206951"/>
-    <hyperlink ref="A58" r:id="rId57" display="http://scicura.org/f/classid=1000206963"/>
-    <hyperlink ref="A59" r:id="rId58" display="http://scicura.org/f/classid=1000206969"/>
-    <hyperlink ref="A60" r:id="rId59" display="http://scicura.org/f/classid=1000206957"/>
-    <hyperlink ref="A61" r:id="rId60" display="http://scicura.org/f/classid=1000281312"/>
-    <hyperlink ref="A62" r:id="rId61" display="http://scicura.org/f/classid=1000281054"/>
-    <hyperlink ref="A63" r:id="rId62" display="http://scicura.org/f/classid=1000281055"/>
-    <hyperlink ref="A64" r:id="rId63" display="http://scicura.org/f/classid=1000281058"/>
-    <hyperlink ref="A65" r:id="rId64" display="http://scicura.org/f/classid=1000281059"/>
-    <hyperlink ref="A66" r:id="rId65" display="http://scicura.org/f/classid=1000281049"/>
-    <hyperlink ref="A67" r:id="rId66" display="http://scicura.org/f/classid=1000281051"/>
-    <hyperlink ref="A68" r:id="rId67" display="http://scicura.org/f/classid=1000281052"/>
-    <hyperlink ref="A69" r:id="rId68" display="http://scicura.org/f/classid=1000281050"/>
-    <hyperlink ref="A70" r:id="rId69" display="http://scicura.org/f/classid=1000206953"/>
-    <hyperlink ref="A71" r:id="rId70" display="http://scicura.org/f/classid=1000206965"/>
-    <hyperlink ref="A72" r:id="rId71" display="http://scicura.org/f/classid=1000206971"/>
-    <hyperlink ref="A73" r:id="rId72" display="http://scicura.org/f/classid=1000206959"/>
-    <hyperlink ref="A74" r:id="rId73" display="http://scicura.org/f/classid=1000281315"/>
-    <hyperlink ref="A75" r:id="rId74" display="http://scicura.org/f/classid=1000206949"/>
-    <hyperlink ref="A76" r:id="rId75" display="http://scicura.org/f/classid=1000206961"/>
-    <hyperlink ref="A77" r:id="rId76" display="http://scicura.org/f/classid=1000206967"/>
-    <hyperlink ref="A78" r:id="rId77" display="http://scicura.org/f/classid=1000206955"/>
-    <hyperlink ref="A79" r:id="rId78" display="http://scicura.org/f/classid=1000206948"/>
-    <hyperlink ref="A80" r:id="rId79" display="http://scicura.org/f/classid=1000206960"/>
-    <hyperlink ref="A81" r:id="rId80" display="http://scicura.org/f/classid=1000206966"/>
-    <hyperlink ref="A82" r:id="rId81" display="http://scicura.org/f/classid=1000206954"/>
-    <hyperlink ref="A83" r:id="rId82" display="http://scicura.org/f/classid=1000281109"/>
-    <hyperlink ref="A84" r:id="rId83" display="http://scicura.org/f/classid=1000281280"/>
-    <hyperlink ref="A85" r:id="rId84" display="http://scicura.org/f/classid=1000206972"/>
-    <hyperlink ref="A86" r:id="rId85" display="http://scicura.org/f/classid=1000206973"/>
-    <hyperlink ref="A87" r:id="rId86" display="http://scicura.org/f/classid=1000206976"/>
-    <hyperlink ref="A88" r:id="rId87" display="http://scicura.org/f/classid=1000206977"/>
-    <hyperlink ref="A89" r:id="rId88" display="http://scicura.org/f/classid=1000281320"/>
-    <hyperlink ref="A90" r:id="rId89" display="http://scicura.org/f/classid=1000280929"/>
-    <hyperlink ref="A91" r:id="rId90" display="http://scicura.org/f/classid=1000280934"/>
-    <hyperlink ref="A92" r:id="rId91" display="http://scicura.org/f/classid=1000280949"/>
-    <hyperlink ref="A93" r:id="rId92" display="http://scicura.org/f/classid=1000280954"/>
-    <hyperlink ref="A94" r:id="rId93" display="http://scicura.org/f/classid=1000280912"/>
-    <hyperlink ref="A95" r:id="rId94" display="http://scicura.org/f/classid=1000280916"/>
-    <hyperlink ref="A96" r:id="rId95" display="http://scicura.org/f/classid=1000280918"/>
-    <hyperlink ref="A97" r:id="rId96" display="http://scicura.org/f/classid=1000280914"/>
-    <hyperlink ref="A98" r:id="rId97" display="http://scicura.org/f/classid=1000281294"/>
-    <hyperlink ref="A99" r:id="rId98" display="http://scicura.org/f/classid=1000280781"/>
-    <hyperlink ref="A100" r:id="rId99" display="http://scicura.org/f/classid=1000280932"/>
-    <hyperlink ref="A101" r:id="rId100" display="http://scicura.org/f/classid=1000280947"/>
-    <hyperlink ref="A102" r:id="rId101" display="http://scicura.org/f/classid=1000280952"/>
-    <hyperlink ref="A103" r:id="rId102" display="http://scicura.org/f/classid=1000206928"/>
-    <hyperlink ref="A104" r:id="rId103" display="http://scicura.org/f/classid=1000206940"/>
-    <hyperlink ref="A105" r:id="rId104" display="http://scicura.org/f/classid=1000206946"/>
-    <hyperlink ref="A106" r:id="rId105" display="http://scicura.org/f/classid=1000206934"/>
-    <hyperlink ref="A107" r:id="rId106" display="http://scicura.org/f/classid=1000281317"/>
-    <hyperlink ref="A108" r:id="rId107" display="http://scicura.org/f/classid=1000280927"/>
-    <hyperlink ref="A109" r:id="rId108" display="http://scicura.org/f/classid=1000280930"/>
-    <hyperlink ref="A110" r:id="rId109" display="http://scicura.org/f/classid=1000280945"/>
-    <hyperlink ref="A111" r:id="rId110" display="http://scicura.org/f/classid=1000280950"/>
-    <hyperlink ref="A112" r:id="rId111" display="http://scicura.org/f/classid=1000206926"/>
-    <hyperlink ref="A113" r:id="rId112" display="http://scicura.org/f/classid=1000206938"/>
-    <hyperlink ref="A114" r:id="rId113" display="http://scicura.org/f/classid=1000206944"/>
-    <hyperlink ref="A115" r:id="rId114" display="http://scicura.org/f/classid=1000281087"/>
-    <hyperlink ref="A116" r:id="rId115" display="http://scicura.org/f/classid=1000206932"/>
-    <hyperlink ref="A117" r:id="rId116" display="http://scicura.org/f/classid=1000280790"/>
-    <hyperlink ref="A118" r:id="rId117" display="http://scicura.org/f/classid=1000280933"/>
-    <hyperlink ref="A119" r:id="rId118" display="http://scicura.org/f/classid=1000280948"/>
-    <hyperlink ref="A120" r:id="rId119" display="http://scicura.org/f/classid=1000280953"/>
-    <hyperlink ref="A121" r:id="rId120" display="http://scicura.org/f/classid=1000280911"/>
-    <hyperlink ref="A122" r:id="rId121" display="http://scicura.org/f/classid=1000280915"/>
-    <hyperlink ref="A123" r:id="rId122" display="http://scicura.org/f/classid=1000280917"/>
-    <hyperlink ref="A124" r:id="rId123" display="http://scicura.org/f/classid=1000280913"/>
-    <hyperlink ref="A125" r:id="rId124" display="http://scicura.org/f/classid=1000280928"/>
-    <hyperlink ref="A126" r:id="rId125" display="http://scicura.org/f/classid=1000280931"/>
-    <hyperlink ref="A127" r:id="rId126" display="http://scicura.org/f/classid=1000280946"/>
-    <hyperlink ref="A128" r:id="rId127" display="http://scicura.org/f/classid=1000280951"/>
-    <hyperlink ref="A129" r:id="rId128" display="http://scicura.org/f/classid=1000206927"/>
-    <hyperlink ref="A130" r:id="rId129" display="http://scicura.org/f/classid=1000206939"/>
-    <hyperlink ref="A131" r:id="rId130" display="http://scicura.org/f/classid=1000206945"/>
-    <hyperlink ref="A132" r:id="rId131" display="http://scicura.org/f/classid=1000206933"/>
-    <hyperlink ref="A133" r:id="rId132" display="http://scicura.org/f/classid=1000281011"/>
-    <hyperlink ref="A134" r:id="rId133" display="http://scicura.org/f/classid=1000281053"/>
-    <hyperlink ref="A135" r:id="rId134" display="http://scicura.org/f/classid=1000281056"/>
-    <hyperlink ref="A136" r:id="rId135" display="http://scicura.org/f/classid=1000281057"/>
-    <hyperlink ref="A137" r:id="rId136" display="http://scicura.org/f/classid=1000281045"/>
-    <hyperlink ref="A138" r:id="rId137" display="http://scicura.org/f/classid=1000281047"/>
-    <hyperlink ref="A139" r:id="rId138" display="http://scicura.org/f/classid=1000281048"/>
-    <hyperlink ref="A140" r:id="rId139" display="http://scicura.org/f/classid=1000281046"/>
-    <hyperlink ref="A141" r:id="rId140" display="http://scicura.org/f/classid=1000281277"/>
-    <hyperlink ref="A142" r:id="rId141" display="http://scicura.org/f/classid=1000206929"/>
-    <hyperlink ref="A143" r:id="rId142" display="http://scicura.org/f/classid=1000206941"/>
-    <hyperlink ref="A144" r:id="rId143" display="http://scicura.org/f/classid=1000206947"/>
-    <hyperlink ref="A145" r:id="rId144" display="http://scicura.org/f/classid=1000206935"/>
-    <hyperlink ref="A146" r:id="rId145" display="http://scicura.org/f/classid=1000206925"/>
-    <hyperlink ref="A147" r:id="rId146" display="http://scicura.org/f/classid=1000206937"/>
-    <hyperlink ref="A148" r:id="rId147" display="http://scicura.org/f/classid=1000206943"/>
-    <hyperlink ref="A149" r:id="rId148" display="http://scicura.org/f/classid=1000206931"/>
-    <hyperlink ref="A150" r:id="rId149" display="http://scicura.org/f/classid=1000206924"/>
-    <hyperlink ref="A151" r:id="rId150" display="http://scicura.org/f/classid=1000206936"/>
-    <hyperlink ref="A152" r:id="rId151" display="http://scicura.org/f/classid=1000206942"/>
-    <hyperlink ref="A153" r:id="rId152" display="http://scicura.org/f/classid=1000206930"/>
-    <hyperlink ref="A154" r:id="rId153" display="http://scicura.org/f/classid=1000280909"/>
-    <hyperlink ref="A155" r:id="rId154" display="http://scicura.org/f/classid=1000280910"/>
-    <hyperlink ref="A156" r:id="rId155" display="http://scicura.org/f/classid=1000280907"/>
-    <hyperlink ref="A157" r:id="rId156" display="http://scicura.org/f/classid=1000280906"/>
-    <hyperlink ref="A158" r:id="rId157" display="http://scicura.org/f/classid=1000280905"/>
-    <hyperlink ref="A159" r:id="rId158" display="http://scicura.org/f/classid=1000280908"/>
-    <hyperlink ref="A160" r:id="rId159" display="http://scicura.org/f/classid=1000280904"/>
-    <hyperlink ref="A161" r:id="rId160" display="http://scicura.org/f/classid=1000280779"/>
-    <hyperlink ref="A162" r:id="rId161" display="http://scicura.org/f/classid=1000281278"/>
-    <hyperlink ref="A163" r:id="rId162" display="http://scicura.org/f/classid=1000280806"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://scicura.org/f/classid=1000206915" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" display="http://scicura.org/f/classid=1000206992" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" display="http://scicura.org/f/classid=1000281286" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" display="http://scicura.org/f/classid=1000206991" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" display="http://scicura.org/f/classid=1000206990" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" display="http://scicura.org/f/classid=1000206922" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" display="http://scicura.org/f/classid=1000206923" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" display="http://scicura.org/f/classid=1000206920" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" display="http://scicura.org/f/classid=1000280758" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" display="http://scicura.org/f/classid=1000206919" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId11" display="http://scicura.org/f/classid=1000206921" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="A13" r:id="rId12" display="http://scicura.org/f/classid=1000206918" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="A14" r:id="rId13" display="http://scicura.org/f/classid=1000206989" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="A15" r:id="rId14" display="http://scicura.org/f/classid=1000206988" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="A16" r:id="rId15" display="http://scicura.org/f/classid=1000206974" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="A17" r:id="rId16" display="http://scicura.org/f/classid=1000206975" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="A18" r:id="rId17" display="http://scicura.org/f/classid=1000206978" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="A19" r:id="rId18" display="http://scicura.org/f/classid=1000206979" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="A20" r:id="rId19" display="http://scicura.org/f/classid=1000281314" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="A21" r:id="rId20" display="http://scicura.org/f/classid=1000280939" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="A22" r:id="rId21" display="http://scicura.org/f/classid=1000280944" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="A23" r:id="rId22" display="http://scicura.org/f/classid=1000280959" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="A24" r:id="rId23" display="http://scicura.org/f/classid=1000280964" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="A25" r:id="rId24" display="http://scicura.org/f/classid=1000280920" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="A26" r:id="rId25" display="http://scicura.org/f/classid=1000280924" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="A27" r:id="rId26" display="http://scicura.org/f/classid=1000280926" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="A28" r:id="rId27" display="http://scicura.org/f/classid=1000280922" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="A29" r:id="rId28" display="http://scicura.org/f/classid=1000280937" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="A30" r:id="rId29" display="http://scicura.org/f/classid=1000280942" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="A31" r:id="rId30" display="http://scicura.org/f/classid=1000280957" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="A32" r:id="rId31" display="http://scicura.org/f/classid=1000280962" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="A33" r:id="rId32" display="http://scicura.org/f/classid=1000206952" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="A34" r:id="rId33" display="http://scicura.org/f/classid=1000206964" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="A35" r:id="rId34" display="http://scicura.org/f/classid=1000206970" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="A36" r:id="rId35" display="http://scicura.org/f/classid=1000206958" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="A37" r:id="rId36" display="http://scicura.org/f/classid=1000280935" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="A38" r:id="rId37" display="http://scicura.org/f/classid=1000280940" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="A39" r:id="rId38" display="http://scicura.org/f/classid=1000280955" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="A40" r:id="rId39" display="http://scicura.org/f/classid=1000280960" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="A41" r:id="rId40" display="http://scicura.org/f/classid=1000206950" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="A42" r:id="rId41" display="http://scicura.org/f/classid=1000206962" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="A43" r:id="rId42" display="http://scicura.org/f/classid=1000206968" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="A44" r:id="rId43" display="http://scicura.org/f/classid=1000206956" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="A45" r:id="rId44" display="http://scicura.org/f/classid=1000280938" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="A46" r:id="rId45" display="http://scicura.org/f/classid=1000280943" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="A47" r:id="rId46" display="http://scicura.org/f/classid=1000280958" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="A48" r:id="rId47" display="http://scicura.org/f/classid=1000280963" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="A49" r:id="rId48" display="http://scicura.org/f/classid=1000280919" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="A50" r:id="rId49" display="http://scicura.org/f/classid=1000280923" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="A51" r:id="rId50" display="http://scicura.org/f/classid=1000280925" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="A52" r:id="rId51" display="http://scicura.org/f/classid=1000280921" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="A53" r:id="rId52" display="http://scicura.org/f/classid=1000280936" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="A54" r:id="rId53" display="http://scicura.org/f/classid=1000280941" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="A55" r:id="rId54" display="http://scicura.org/f/classid=1000280956" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="A56" r:id="rId55" display="http://scicura.org/f/classid=1000280961" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="A57" r:id="rId56" display="http://scicura.org/f/classid=1000206951" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="A58" r:id="rId57" display="http://scicura.org/f/classid=1000206963" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="A59" r:id="rId58" display="http://scicura.org/f/classid=1000206969" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="A60" r:id="rId59" display="http://scicura.org/f/classid=1000206957" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="A61" r:id="rId60" display="http://scicura.org/f/classid=1000281312" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="A62" r:id="rId61" display="http://scicura.org/f/classid=1000281054" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="A63" r:id="rId62" display="http://scicura.org/f/classid=1000281055" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="A64" r:id="rId63" display="http://scicura.org/f/classid=1000281058" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="A65" r:id="rId64" display="http://scicura.org/f/classid=1000281059" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="A66" r:id="rId65" display="http://scicura.org/f/classid=1000281049" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="A67" r:id="rId66" display="http://scicura.org/f/classid=1000281051" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="A68" r:id="rId67" display="http://scicura.org/f/classid=1000281052" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="A69" r:id="rId68" display="http://scicura.org/f/classid=1000281050" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="A70" r:id="rId69" display="http://scicura.org/f/classid=1000206953" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="A71" r:id="rId70" display="http://scicura.org/f/classid=1000206965" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="A72" r:id="rId71" display="http://scicura.org/f/classid=1000206971" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="A73" r:id="rId72" display="http://scicura.org/f/classid=1000206959" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="A74" r:id="rId73" display="http://scicura.org/f/classid=1000281315" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="A75" r:id="rId74" display="http://scicura.org/f/classid=1000206949" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="A76" r:id="rId75" display="http://scicura.org/f/classid=1000206961" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="A77" r:id="rId76" display="http://scicura.org/f/classid=1000206967" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="A78" r:id="rId77" display="http://scicura.org/f/classid=1000206955" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="A79" r:id="rId78" display="http://scicura.org/f/classid=1000206948" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="A80" r:id="rId79" display="http://scicura.org/f/classid=1000206960" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="A81" r:id="rId80" display="http://scicura.org/f/classid=1000206966" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="A82" r:id="rId81" display="http://scicura.org/f/classid=1000206954" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="A83" r:id="rId82" display="http://scicura.org/f/classid=1000281109" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="A84" r:id="rId83" display="http://scicura.org/f/classid=1000281280" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="A85" r:id="rId84" display="http://scicura.org/f/classid=1000206972" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="A86" r:id="rId85" display="http://scicura.org/f/classid=1000206973" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="A87" r:id="rId86" display="http://scicura.org/f/classid=1000206976" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="A88" r:id="rId87" display="http://scicura.org/f/classid=1000206977" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="A89" r:id="rId88" display="http://scicura.org/f/classid=1000281320" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="A90" r:id="rId89" display="http://scicura.org/f/classid=1000280929" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="A91" r:id="rId90" display="http://scicura.org/f/classid=1000280934" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="A92" r:id="rId91" display="http://scicura.org/f/classid=1000280949" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="A93" r:id="rId92" display="http://scicura.org/f/classid=1000280954" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="A94" r:id="rId93" display="http://scicura.org/f/classid=1000280912" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="A95" r:id="rId94" display="http://scicura.org/f/classid=1000280916" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="A96" r:id="rId95" display="http://scicura.org/f/classid=1000280918" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="A97" r:id="rId96" display="http://scicura.org/f/classid=1000280914" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="A98" r:id="rId97" display="http://scicura.org/f/classid=1000281294" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="A99" r:id="rId98" display="http://scicura.org/f/classid=1000280781" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="A100" r:id="rId99" display="http://scicura.org/f/classid=1000280932" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="A101" r:id="rId100" display="http://scicura.org/f/classid=1000280947" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="A102" r:id="rId101" display="http://scicura.org/f/classid=1000280952" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="A103" r:id="rId102" display="http://scicura.org/f/classid=1000206928" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="A104" r:id="rId103" display="http://scicura.org/f/classid=1000206940" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="A105" r:id="rId104" display="http://scicura.org/f/classid=1000206946" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="A106" r:id="rId105" display="http://scicura.org/f/classid=1000206934" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="A107" r:id="rId106" display="http://scicura.org/f/classid=1000281317" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="A108" r:id="rId107" display="http://scicura.org/f/classid=1000280927" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="A109" r:id="rId108" display="http://scicura.org/f/classid=1000280930" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="A110" r:id="rId109" display="http://scicura.org/f/classid=1000280945" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="A111" r:id="rId110" display="http://scicura.org/f/classid=1000280950" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
+    <hyperlink ref="A112" r:id="rId111" display="http://scicura.org/f/classid=1000206926" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
+    <hyperlink ref="A113" r:id="rId112" display="http://scicura.org/f/classid=1000206938" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
+    <hyperlink ref="A114" r:id="rId113" display="http://scicura.org/f/classid=1000206944" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
+    <hyperlink ref="A115" r:id="rId114" display="http://scicura.org/f/classid=1000281087" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
+    <hyperlink ref="A116" r:id="rId115" display="http://scicura.org/f/classid=1000206932" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
+    <hyperlink ref="A117" r:id="rId116" display="http://scicura.org/f/classid=1000280790" xr:uid="{00000000-0004-0000-0100-000073000000}"/>
+    <hyperlink ref="A118" r:id="rId117" display="http://scicura.org/f/classid=1000280933" xr:uid="{00000000-0004-0000-0100-000074000000}"/>
+    <hyperlink ref="A119" r:id="rId118" display="http://scicura.org/f/classid=1000280948" xr:uid="{00000000-0004-0000-0100-000075000000}"/>
+    <hyperlink ref="A120" r:id="rId119" display="http://scicura.org/f/classid=1000280953" xr:uid="{00000000-0004-0000-0100-000076000000}"/>
+    <hyperlink ref="A121" r:id="rId120" display="http://scicura.org/f/classid=1000280911" xr:uid="{00000000-0004-0000-0100-000077000000}"/>
+    <hyperlink ref="A122" r:id="rId121" display="http://scicura.org/f/classid=1000280915" xr:uid="{00000000-0004-0000-0100-000078000000}"/>
+    <hyperlink ref="A123" r:id="rId122" display="http://scicura.org/f/classid=1000280917" xr:uid="{00000000-0004-0000-0100-000079000000}"/>
+    <hyperlink ref="A124" r:id="rId123" display="http://scicura.org/f/classid=1000280913" xr:uid="{00000000-0004-0000-0100-00007A000000}"/>
+    <hyperlink ref="A125" r:id="rId124" display="http://scicura.org/f/classid=1000280928" xr:uid="{00000000-0004-0000-0100-00007B000000}"/>
+    <hyperlink ref="A126" r:id="rId125" display="http://scicura.org/f/classid=1000280931" xr:uid="{00000000-0004-0000-0100-00007C000000}"/>
+    <hyperlink ref="A127" r:id="rId126" display="http://scicura.org/f/classid=1000280946" xr:uid="{00000000-0004-0000-0100-00007D000000}"/>
+    <hyperlink ref="A128" r:id="rId127" display="http://scicura.org/f/classid=1000280951" xr:uid="{00000000-0004-0000-0100-00007E000000}"/>
+    <hyperlink ref="A129" r:id="rId128" display="http://scicura.org/f/classid=1000206927" xr:uid="{00000000-0004-0000-0100-00007F000000}"/>
+    <hyperlink ref="A130" r:id="rId129" display="http://scicura.org/f/classid=1000206939" xr:uid="{00000000-0004-0000-0100-000080000000}"/>
+    <hyperlink ref="A131" r:id="rId130" display="http://scicura.org/f/classid=1000206945" xr:uid="{00000000-0004-0000-0100-000081000000}"/>
+    <hyperlink ref="A132" r:id="rId131" display="http://scicura.org/f/classid=1000206933" xr:uid="{00000000-0004-0000-0100-000082000000}"/>
+    <hyperlink ref="A133" r:id="rId132" display="http://scicura.org/f/classid=1000281011" xr:uid="{00000000-0004-0000-0100-000083000000}"/>
+    <hyperlink ref="A134" r:id="rId133" display="http://scicura.org/f/classid=1000281053" xr:uid="{00000000-0004-0000-0100-000084000000}"/>
+    <hyperlink ref="A135" r:id="rId134" display="http://scicura.org/f/classid=1000281056" xr:uid="{00000000-0004-0000-0100-000085000000}"/>
+    <hyperlink ref="A136" r:id="rId135" display="http://scicura.org/f/classid=1000281057" xr:uid="{00000000-0004-0000-0100-000086000000}"/>
+    <hyperlink ref="A137" r:id="rId136" display="http://scicura.org/f/classid=1000281045" xr:uid="{00000000-0004-0000-0100-000087000000}"/>
+    <hyperlink ref="A138" r:id="rId137" display="http://scicura.org/f/classid=1000281047" xr:uid="{00000000-0004-0000-0100-000088000000}"/>
+    <hyperlink ref="A139" r:id="rId138" display="http://scicura.org/f/classid=1000281048" xr:uid="{00000000-0004-0000-0100-000089000000}"/>
+    <hyperlink ref="A140" r:id="rId139" display="http://scicura.org/f/classid=1000281046" xr:uid="{00000000-0004-0000-0100-00008A000000}"/>
+    <hyperlink ref="A141" r:id="rId140" display="http://scicura.org/f/classid=1000281277" xr:uid="{00000000-0004-0000-0100-00008B000000}"/>
+    <hyperlink ref="A142" r:id="rId141" display="http://scicura.org/f/classid=1000206929" xr:uid="{00000000-0004-0000-0100-00008C000000}"/>
+    <hyperlink ref="A143" r:id="rId142" display="http://scicura.org/f/classid=1000206941" xr:uid="{00000000-0004-0000-0100-00008D000000}"/>
+    <hyperlink ref="A144" r:id="rId143" display="http://scicura.org/f/classid=1000206947" xr:uid="{00000000-0004-0000-0100-00008E000000}"/>
+    <hyperlink ref="A145" r:id="rId144" display="http://scicura.org/f/classid=1000206935" xr:uid="{00000000-0004-0000-0100-00008F000000}"/>
+    <hyperlink ref="A146" r:id="rId145" display="http://scicura.org/f/classid=1000206925" xr:uid="{00000000-0004-0000-0100-000090000000}"/>
+    <hyperlink ref="A147" r:id="rId146" display="http://scicura.org/f/classid=1000206937" xr:uid="{00000000-0004-0000-0100-000091000000}"/>
+    <hyperlink ref="A148" r:id="rId147" display="http://scicura.org/f/classid=1000206943" xr:uid="{00000000-0004-0000-0100-000092000000}"/>
+    <hyperlink ref="A149" r:id="rId148" display="http://scicura.org/f/classid=1000206931" xr:uid="{00000000-0004-0000-0100-000093000000}"/>
+    <hyperlink ref="A150" r:id="rId149" display="http://scicura.org/f/classid=1000206924" xr:uid="{00000000-0004-0000-0100-000094000000}"/>
+    <hyperlink ref="A151" r:id="rId150" display="http://scicura.org/f/classid=1000206936" xr:uid="{00000000-0004-0000-0100-000095000000}"/>
+    <hyperlink ref="A152" r:id="rId151" display="http://scicura.org/f/classid=1000206942" xr:uid="{00000000-0004-0000-0100-000096000000}"/>
+    <hyperlink ref="A153" r:id="rId152" display="http://scicura.org/f/classid=1000206930" xr:uid="{00000000-0004-0000-0100-000097000000}"/>
+    <hyperlink ref="A154" r:id="rId153" display="http://scicura.org/f/classid=1000280909" xr:uid="{00000000-0004-0000-0100-000098000000}"/>
+    <hyperlink ref="A155" r:id="rId154" display="http://scicura.org/f/classid=1000280910" xr:uid="{00000000-0004-0000-0100-000099000000}"/>
+    <hyperlink ref="A156" r:id="rId155" display="http://scicura.org/f/classid=1000280907" xr:uid="{00000000-0004-0000-0100-00009A000000}"/>
+    <hyperlink ref="A157" r:id="rId156" display="http://scicura.org/f/classid=1000280906" xr:uid="{00000000-0004-0000-0100-00009B000000}"/>
+    <hyperlink ref="A158" r:id="rId157" display="http://scicura.org/f/classid=1000280905" xr:uid="{00000000-0004-0000-0100-00009C000000}"/>
+    <hyperlink ref="A159" r:id="rId158" display="http://scicura.org/f/classid=1000280908" xr:uid="{00000000-0004-0000-0100-00009D000000}"/>
+    <hyperlink ref="A160" r:id="rId159" display="http://scicura.org/f/classid=1000280904" xr:uid="{00000000-0004-0000-0100-00009E000000}"/>
+    <hyperlink ref="A161" r:id="rId160" display="http://scicura.org/f/classid=1000280779" xr:uid="{00000000-0004-0000-0100-00009F000000}"/>
+    <hyperlink ref="A162" r:id="rId161" display="http://scicura.org/f/classid=1000281278" xr:uid="{00000000-0004-0000-0100-0000A0000000}"/>
+    <hyperlink ref="A163" r:id="rId162" display="http://scicura.org/f/classid=1000280806" xr:uid="{00000000-0004-0000-0100-0000A1000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4525,16 +4520,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4542,10 +4537,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4553,10 +4548,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4564,10 +4559,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4575,21 +4570,21 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4597,10 +4592,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4608,10 +4603,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4619,16 +4614,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D9" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E9" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4636,71 +4631,71 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D10" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E10" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -4709,7 +4704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4764,7 +4759,7 @@
     </row>
     <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -4791,7 +4786,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4799,12 +4794,12 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -4812,7 +4807,7 @@
     </row>
     <row r="12" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>10</v>
@@ -4820,7 +4815,7 @@
     </row>
     <row r="13" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>10</v>
@@ -4828,7 +4823,7 @@
     </row>
     <row r="14" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>10</v>
@@ -4836,7 +4831,7 @@
     </row>
     <row r="15" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>10</v>
@@ -4848,7 +4843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4903,7 +4898,7 @@
     </row>
     <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B6" t="s">
         <v>176</v>
@@ -4943,7 +4938,7 @@
     </row>
     <row r="11" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>177</v>
@@ -4951,7 +4946,7 @@
     </row>
     <row r="12" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>177</v>
@@ -4959,7 +4954,7 @@
     </row>
     <row r="13" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>177</v>
@@ -4967,7 +4962,7 @@
     </row>
     <row r="14" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B14" t="s">
         <v>176</v>
@@ -4975,7 +4970,7 @@
     </row>
     <row r="15" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B15" t="s">
         <v>176</v>
@@ -4987,11 +4982,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5004,13 +4999,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" t="s">
         <v>347</v>
       </c>
-      <c r="B1" t="s">
-        <v>348</v>
-      </c>
       <c r="C1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5021,7 +5016,7 @@
         <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -5032,7 +5027,7 @@
         <v>181</v>
       </c>
       <c r="C3" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -5043,7 +5038,7 @@
         <v>238</v>
       </c>
       <c r="C4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -5054,7 +5049,7 @@
         <v>240</v>
       </c>
       <c r="C5" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -5065,7 +5060,7 @@
         <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -5076,7 +5071,7 @@
         <v>217</v>
       </c>
       <c r="C7" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -5087,7 +5082,7 @@
         <v>242</v>
       </c>
       <c r="C8" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -5098,7 +5093,7 @@
         <v>185</v>
       </c>
       <c r="C9" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -5109,7 +5104,7 @@
         <v>219</v>
       </c>
       <c r="C10" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -5120,7 +5115,7 @@
         <v>244</v>
       </c>
       <c r="C11" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -5131,7 +5126,7 @@
         <v>187</v>
       </c>
       <c r="C12" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -5139,10 +5134,10 @@
         <v>245</v>
       </c>
       <c r="B13" t="s">
-        <v>246</v>
+        <v>513</v>
       </c>
       <c r="C13" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -5153,7 +5148,7 @@
         <v>189</v>
       </c>
       <c r="C14" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -5164,29 +5159,29 @@
         <v>191</v>
       </c>
       <c r="C15" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" t="s">
         <v>247</v>
       </c>
-      <c r="B16" t="s">
-        <v>248</v>
-      </c>
       <c r="C16" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B17" t="s">
         <v>249</v>
       </c>
-      <c r="B17" t="s">
-        <v>250</v>
-      </c>
       <c r="C17" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -5197,18 +5192,18 @@
         <v>193</v>
       </c>
       <c r="C18" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B19" t="s">
         <v>251</v>
       </c>
-      <c r="B19" t="s">
-        <v>252</v>
-      </c>
       <c r="C19" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -5219,40 +5214,40 @@
         <v>195</v>
       </c>
       <c r="C20" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>252</v>
+      </c>
+      <c r="B21" t="s">
         <v>253</v>
       </c>
-      <c r="B21" t="s">
-        <v>254</v>
-      </c>
       <c r="C21" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22" t="s">
         <v>255</v>
       </c>
-      <c r="B22" t="s">
-        <v>256</v>
-      </c>
       <c r="C22" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" t="s">
         <v>257</v>
       </c>
-      <c r="B23" t="s">
-        <v>258</v>
-      </c>
       <c r="C23" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -5263,62 +5258,62 @@
         <v>221</v>
       </c>
       <c r="C24" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>258</v>
+      </c>
+      <c r="B25" t="s">
         <v>259</v>
       </c>
-      <c r="B25" t="s">
-        <v>260</v>
-      </c>
       <c r="C25" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>260</v>
+      </c>
+      <c r="B26" t="s">
         <v>261</v>
       </c>
-      <c r="B26" t="s">
-        <v>262</v>
-      </c>
       <c r="C26" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>262</v>
+      </c>
+      <c r="B27" t="s">
         <v>263</v>
       </c>
-      <c r="B27" t="s">
-        <v>264</v>
-      </c>
       <c r="C27" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>264</v>
+      </c>
+      <c r="B28" t="s">
         <v>265</v>
       </c>
-      <c r="B28" t="s">
-        <v>266</v>
-      </c>
       <c r="C28" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" t="s">
         <v>267</v>
       </c>
-      <c r="B29" t="s">
-        <v>268</v>
-      </c>
       <c r="C29" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -5329,7 +5324,7 @@
         <v>197</v>
       </c>
       <c r="C30" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -5340,73 +5335,73 @@
         <v>199</v>
       </c>
       <c r="C31" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>268</v>
+      </c>
+      <c r="B32" t="s">
         <v>269</v>
       </c>
-      <c r="B32" t="s">
-        <v>270</v>
-      </c>
       <c r="C32" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>270</v>
+      </c>
+      <c r="B33" t="s">
         <v>271</v>
       </c>
-      <c r="B33" t="s">
-        <v>272</v>
-      </c>
       <c r="C33" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>272</v>
+      </c>
+      <c r="B34" t="s">
         <v>273</v>
       </c>
-      <c r="B34" t="s">
-        <v>274</v>
-      </c>
       <c r="C34" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>274</v>
+      </c>
+      <c r="B35" t="s">
         <v>275</v>
       </c>
-      <c r="B35" t="s">
-        <v>276</v>
-      </c>
       <c r="C35" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>276</v>
+      </c>
+      <c r="B36" t="s">
         <v>277</v>
       </c>
-      <c r="B36" t="s">
-        <v>278</v>
-      </c>
       <c r="C36" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>278</v>
+      </c>
+      <c r="B37" t="s">
         <v>279</v>
       </c>
-      <c r="B37" t="s">
-        <v>280</v>
-      </c>
       <c r="C37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -5417,29 +5412,29 @@
         <v>223</v>
       </c>
       <c r="C38" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>280</v>
+      </c>
+      <c r="B39" t="s">
         <v>281</v>
       </c>
-      <c r="B39" t="s">
-        <v>282</v>
-      </c>
       <c r="C39" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B40" t="s">
         <v>283</v>
       </c>
-      <c r="B40" t="s">
-        <v>284</v>
-      </c>
       <c r="C40" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -5450,18 +5445,18 @@
         <v>225</v>
       </c>
       <c r="C41" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B42" t="s">
         <v>285</v>
       </c>
-      <c r="B42" t="s">
-        <v>286</v>
-      </c>
       <c r="C42" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -5472,62 +5467,62 @@
         <v>201</v>
       </c>
       <c r="C43" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>286</v>
+      </c>
+      <c r="B44" t="s">
         <v>287</v>
       </c>
-      <c r="B44" t="s">
-        <v>288</v>
-      </c>
       <c r="C44" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>288</v>
+      </c>
+      <c r="B45" t="s">
         <v>289</v>
       </c>
-      <c r="B45" t="s">
-        <v>290</v>
-      </c>
       <c r="C45" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>290</v>
+      </c>
+      <c r="B46" t="s">
         <v>291</v>
       </c>
-      <c r="B46" t="s">
-        <v>292</v>
-      </c>
       <c r="C46" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>292</v>
+      </c>
+      <c r="B47" t="s">
         <v>293</v>
       </c>
-      <c r="B47" t="s">
-        <v>294</v>
-      </c>
       <c r="C47" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>294</v>
+      </c>
+      <c r="B48" t="s">
         <v>295</v>
       </c>
-      <c r="B48" t="s">
-        <v>296</v>
-      </c>
       <c r="C48" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -5538,29 +5533,29 @@
         <v>203</v>
       </c>
       <c r="C49" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>296</v>
+      </c>
+      <c r="B50" t="s">
         <v>297</v>
       </c>
-      <c r="B50" t="s">
-        <v>298</v>
-      </c>
       <c r="C50" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>298</v>
+      </c>
+      <c r="B51" t="s">
         <v>299</v>
       </c>
-      <c r="B51" t="s">
-        <v>300</v>
-      </c>
       <c r="C51" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -5571,95 +5566,95 @@
         <v>205</v>
       </c>
       <c r="C52" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>300</v>
+      </c>
+      <c r="B53" t="s">
         <v>301</v>
       </c>
-      <c r="B53" t="s">
-        <v>302</v>
-      </c>
       <c r="C53" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>302</v>
+      </c>
+      <c r="B54" t="s">
         <v>303</v>
       </c>
-      <c r="B54" t="s">
-        <v>304</v>
-      </c>
       <c r="C54" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>304</v>
+      </c>
+      <c r="B55" t="s">
         <v>305</v>
       </c>
-      <c r="B55" t="s">
-        <v>306</v>
-      </c>
       <c r="C55" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>306</v>
+      </c>
+      <c r="B56" t="s">
         <v>307</v>
       </c>
-      <c r="B56" t="s">
-        <v>308</v>
-      </c>
       <c r="C56" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>308</v>
+      </c>
+      <c r="B57" t="s">
         <v>309</v>
       </c>
-      <c r="B57" t="s">
-        <v>310</v>
-      </c>
       <c r="C57" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>310</v>
+      </c>
+      <c r="B58" t="s">
         <v>311</v>
       </c>
-      <c r="B58" t="s">
-        <v>312</v>
-      </c>
       <c r="C58" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>312</v>
+      </c>
+      <c r="B59" t="s">
         <v>313</v>
       </c>
-      <c r="B59" t="s">
-        <v>314</v>
-      </c>
       <c r="C59" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>314</v>
+      </c>
+      <c r="B60" t="s">
         <v>315</v>
       </c>
-      <c r="B60" t="s">
-        <v>316</v>
-      </c>
       <c r="C60" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -5670,7 +5665,7 @@
         <v>207</v>
       </c>
       <c r="C61" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -5681,7 +5676,7 @@
         <v>227</v>
       </c>
       <c r="C62" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -5692,7 +5687,7 @@
         <v>209</v>
       </c>
       <c r="C63" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -5703,7 +5698,7 @@
         <v>229</v>
       </c>
       <c r="C64" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -5714,7 +5709,7 @@
         <v>211</v>
       </c>
       <c r="C65" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -5725,29 +5720,29 @@
         <v>213</v>
       </c>
       <c r="C66" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>316</v>
+      </c>
+      <c r="B67" t="s">
         <v>317</v>
       </c>
-      <c r="B67" t="s">
-        <v>318</v>
-      </c>
       <c r="C67" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>318</v>
+      </c>
+      <c r="B68" t="s">
         <v>319</v>
       </c>
-      <c r="B68" t="s">
-        <v>320</v>
-      </c>
       <c r="C68" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -5758,73 +5753,73 @@
         <v>231</v>
       </c>
       <c r="C69" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>320</v>
+      </c>
+      <c r="B70" t="s">
         <v>321</v>
       </c>
-      <c r="B70" t="s">
-        <v>322</v>
-      </c>
       <c r="C70" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>322</v>
+      </c>
+      <c r="B71" t="s">
         <v>323</v>
       </c>
-      <c r="B71" t="s">
-        <v>324</v>
-      </c>
       <c r="C71" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>324</v>
+      </c>
+      <c r="B72" t="s">
         <v>325</v>
       </c>
-      <c r="B72" t="s">
-        <v>326</v>
-      </c>
       <c r="C72" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>326</v>
+      </c>
+      <c r="B73" t="s">
         <v>327</v>
       </c>
-      <c r="B73" t="s">
-        <v>328</v>
-      </c>
       <c r="C73" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>328</v>
+      </c>
+      <c r="B74" t="s">
         <v>329</v>
       </c>
-      <c r="B74" t="s">
-        <v>330</v>
-      </c>
       <c r="C74" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>330</v>
+      </c>
+      <c r="B75" t="s">
         <v>331</v>
       </c>
-      <c r="B75" t="s">
-        <v>332</v>
-      </c>
       <c r="C75" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -5835,29 +5830,29 @@
         <v>233</v>
       </c>
       <c r="C76" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>332</v>
+      </c>
+      <c r="B77" t="s">
         <v>333</v>
       </c>
-      <c r="B77" t="s">
-        <v>334</v>
-      </c>
       <c r="C77" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>334</v>
+      </c>
+      <c r="B78" t="s">
         <v>335</v>
       </c>
-      <c r="B78" t="s">
-        <v>336</v>
-      </c>
       <c r="C78" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -5868,7 +5863,7 @@
         <v>235</v>
       </c>
       <c r="C79" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -5879,51 +5874,51 @@
         <v>236</v>
       </c>
       <c r="C80" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>336</v>
+      </c>
+      <c r="B81" t="s">
         <v>337</v>
       </c>
-      <c r="B81" t="s">
-        <v>338</v>
-      </c>
       <c r="C81" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>338</v>
+      </c>
+      <c r="B82" t="s">
         <v>339</v>
       </c>
-      <c r="B82" t="s">
-        <v>340</v>
-      </c>
       <c r="C82" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>342</v>
+      </c>
+      <c r="B83" t="s">
         <v>343</v>
       </c>
-      <c r="B83" t="s">
-        <v>344</v>
-      </c>
       <c r="C83" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>340</v>
+      </c>
+      <c r="B84" t="s">
         <v>341</v>
       </c>
-      <c r="B84" t="s">
-        <v>342</v>
-      </c>
       <c r="C84" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -5934,18 +5929,18 @@
         <v>215</v>
       </c>
       <c r="C85" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>344</v>
+      </c>
+      <c r="B86" t="s">
         <v>345</v>
       </c>
-      <c r="B86" t="s">
-        <v>346</v>
-      </c>
       <c r="C86" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>